<commit_message>
fix labels; incorrect parents
- fixes labels where there was no space between words, e.g.
  "GovernmentalOrganisation" should be "Governmental Organisation"
- fixes are across entities (organisations, authorities, data subjects),
  processing scales
- in dpv-pd, GeneticData has parent fixed to dpv-pd:Health (thanks to
  @besteves4) and all suffixes of -Data have been removed since the
  concepts are already in PD namespace
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/dpv-pd.xlsx
+++ b/documentation-generator/vocab_csv/dpv-pd.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="754">
   <si>
     <t>Term</t>
   </si>
@@ -1292,16 +1292,13 @@
     <t>Information about reputation in the public sphere</t>
   </si>
   <si>
-    <t>GeneticData</t>
-  </si>
-  <si>
-    <t>Genetic Data</t>
+    <t>Genetic</t>
   </si>
   <si>
     <t>Information about inherited or acquired genetic characteristics</t>
   </si>
   <si>
-    <t>dpv:HealthData</t>
+    <t>dpv-pd:Health</t>
   </si>
   <si>
     <t>https://www.w3.org/community/dpvcg/wiki/MinutesOfMeeting_20220518</t>
@@ -1382,10 +1379,7 @@
     <t>Information about historical data related to or relevant regarding history or past events</t>
   </si>
   <si>
-    <t>HouseholdData</t>
-  </si>
-  <si>
-    <t>Household Data</t>
+    <t>Household</t>
   </si>
   <si>
     <t>Information about personal or household activities</t>
@@ -1599,9 +1593,6 @@
   </si>
   <si>
     <t>Information about mental health.</t>
-  </si>
-  <si>
-    <t>dpv-pd:Health</t>
   </si>
   <si>
     <t>Name</t>
@@ -1982,16 +1973,16 @@
     <t>Information about public life</t>
   </si>
   <si>
-    <t>PubliclyAvailableSocialMediaData</t>
-  </si>
-  <si>
-    <t>Publicly Available Social Media Data</t>
+    <t>PubliclyAvailableSocialMedia</t>
+  </si>
+  <si>
+    <t>Publicly Available Social Media</t>
   </si>
   <si>
     <t>Information about social media that is publicly available</t>
   </si>
   <si>
-    <t>dpv-pd:SocialMediaData</t>
+    <t>dpv-pd:SocialMedia</t>
   </si>
   <si>
     <t>Purchase</t>
@@ -2178,10 +2169,10 @@
     <t>svd:Social</t>
   </si>
   <si>
-    <t>SocialMediaData</t>
-  </si>
-  <si>
-    <t>Social Media Data</t>
+    <t>SocialMedia</t>
+  </si>
+  <si>
+    <t>Social Media</t>
   </si>
   <si>
     <t>Information about social media</t>
@@ -2344,10 +2335,7 @@
     <t>Information about vehicle license registration</t>
   </si>
   <si>
-    <t>VehicleData</t>
-  </si>
-  <si>
-    <t>Vehicle Data</t>
+    <t>Vehicle</t>
   </si>
   <si>
     <t>Information about vehicles</t>
@@ -2362,19 +2350,19 @@
     <t>Information about vehicle license</t>
   </si>
   <si>
-    <t>dpv-pd:Identifying,dpv-pd:VehicleData</t>
-  </si>
-  <si>
-    <t>VehicleUsageData</t>
-  </si>
-  <si>
-    <t>Vehicle Usage Data</t>
+    <t>dpv-pd:Identifying,dpv-pd:Vehicle</t>
+  </si>
+  <si>
+    <t>VehicleUsage</t>
+  </si>
+  <si>
+    <t>Vehicle Usage</t>
   </si>
   <si>
     <t>Information about usage of vehicles, e.g. driving statistics</t>
   </si>
   <si>
-    <t>dpv-pd:VehicleData,dpv-pd:Behavioral</t>
+    <t>dpv-pd:Vehicle,dpv-pd:Behavioral</t>
   </si>
   <si>
     <t>VoiceCommunicationRecording</t>
@@ -9752,7 +9740,7 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="29.88"/>
     <col customWidth="1" min="3" max="3" width="54.25"/>
-    <col customWidth="1" min="4" max="4" width="35.88"/>
+    <col customWidth="1" min="4" max="4" width="61.63"/>
     <col customWidth="1" min="10" max="10" width="67.5"/>
   </cols>
   <sheetData>
@@ -13990,13 +13978,13 @@
         <v>395</v>
       </c>
       <c r="B86" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="C86" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="D86" s="10" t="s">
         <v>397</v>
-      </c>
-      <c r="D86" s="10" t="s">
-        <v>398</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>19</v>
@@ -14017,7 +14005,7 @@
         <v>30</v>
       </c>
       <c r="O86" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P86" s="12"/>
       <c r="Q86" s="12"/>
@@ -14035,16 +14023,16 @@
     </row>
     <row r="87">
       <c r="A87" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="C87" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="B87" s="16" t="s">
-        <v>400</v>
-      </c>
-      <c r="C87" s="32" t="s">
+      <c r="D87" s="10" t="s">
         <v>401</v>
-      </c>
-      <c r="D87" s="10" t="s">
-        <v>402</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>19</v>
@@ -14085,13 +14073,13 @@
     </row>
     <row r="88">
       <c r="A88" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="B88" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="C88" s="10" t="s">
         <v>404</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>405</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>170</v>
@@ -14135,13 +14123,13 @@
     </row>
     <row r="89">
       <c r="A89" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="B89" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="C89" s="10" t="s">
         <v>407</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>408</v>
       </c>
       <c r="D89" s="10" t="s">
         <v>124</v>
@@ -14185,13 +14173,13 @@
     </row>
     <row r="90">
       <c r="A90" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="B90" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="B90" s="16" t="s">
+      <c r="C90" s="31" t="s">
         <v>410</v>
-      </c>
-      <c r="C90" s="31" t="s">
-        <v>411</v>
       </c>
       <c r="D90" s="10" t="s">
         <v>127</v>
@@ -14235,13 +14223,13 @@
     </row>
     <row r="91">
       <c r="A91" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="C91" s="32" t="s">
         <v>412</v>
-      </c>
-      <c r="B91" s="16" t="s">
-        <v>412</v>
-      </c>
-      <c r="C91" s="32" t="s">
-        <v>413</v>
       </c>
       <c r="D91" s="10" t="s">
         <v>174</v>
@@ -14251,7 +14239,7 @@
       </c>
       <c r="F91" s="12"/>
       <c r="G91" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="12"/>
@@ -14287,13 +14275,13 @@
     </row>
     <row r="92">
       <c r="A92" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="B92" s="16" t="s">
         <v>415</v>
       </c>
-      <c r="B92" s="16" t="s">
+      <c r="C92" s="10" t="s">
         <v>416</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>417</v>
       </c>
       <c r="D92" s="10" t="s">
         <v>174</v>
@@ -14337,13 +14325,13 @@
     </row>
     <row r="93">
       <c r="A93" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="B93" s="16" t="s">
         <v>418</v>
       </c>
-      <c r="B93" s="16" t="s">
+      <c r="C93" s="10" t="s">
         <v>419</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>420</v>
       </c>
       <c r="D93" s="10" t="s">
         <v>174</v>
@@ -14387,13 +14375,13 @@
     </row>
     <row r="94">
       <c r="A94" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C94" s="31" t="s">
         <v>421</v>
-      </c>
-      <c r="B94" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C94" s="31" t="s">
-        <v>422</v>
       </c>
       <c r="D94" s="10" t="s">
         <v>127</v>
@@ -14437,13 +14425,13 @@
     </row>
     <row r="95">
       <c r="A95" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>422</v>
+      </c>
+      <c r="C95" s="10" t="s">
         <v>423</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>423</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>424</v>
       </c>
       <c r="D95" s="10" t="s">
         <v>34</v>
@@ -14487,13 +14475,13 @@
     </row>
     <row r="96">
       <c r="A96" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="C96" s="10" t="s">
         <v>425</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>427</v>
       </c>
       <c r="D96" s="10" t="s">
         <v>34</v>
@@ -14535,13 +14523,13 @@
     </row>
     <row r="97">
       <c r="A97" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="C97" s="10" t="s">
         <v>428</v>
-      </c>
-      <c r="B97" s="16" t="s">
-        <v>429</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>430</v>
       </c>
       <c r="D97" s="10" t="s">
         <v>198</v>
@@ -14585,13 +14573,13 @@
     </row>
     <row r="98">
       <c r="A98" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="C98" s="10" t="s">
         <v>431</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>432</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>433</v>
       </c>
       <c r="D98" s="10" t="s">
         <v>260</v>
@@ -14633,13 +14621,13 @@
     </row>
     <row r="99">
       <c r="A99" s="10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D99" s="10" t="s">
         <v>213</v>
@@ -14681,13 +14669,13 @@
     </row>
     <row r="100">
       <c r="A100" s="10" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>159</v>
@@ -14731,13 +14719,13 @@
     </row>
     <row r="101">
       <c r="A101" s="10" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D101" s="10" t="s">
         <v>219</v>
@@ -14781,16 +14769,16 @@
     </row>
     <row r="102">
       <c r="A102" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>439</v>
+      </c>
+      <c r="C102" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="B102" s="16" t="s">
-        <v>441</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>442</v>
-      </c>
       <c r="D102" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E102" s="10" t="s">
         <v>19</v>
@@ -14831,13 +14819,13 @@
     </row>
     <row r="103">
       <c r="A103" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="C103" s="10" t="s">
         <v>443</v>
-      </c>
-      <c r="B103" s="16" t="s">
-        <v>444</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>445</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>351</v>
@@ -14881,13 +14869,13 @@
     </row>
     <row r="104">
       <c r="A104" s="10" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D104" s="10" t="s">
         <v>378</v>
@@ -14929,13 +14917,13 @@
     </row>
     <row r="105">
       <c r="A105" s="10" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D105" s="10" t="s">
         <v>358</v>
@@ -14979,13 +14967,13 @@
     </row>
     <row r="106">
       <c r="A106" s="10" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D106" s="10" t="s">
         <v>201</v>
@@ -15029,13 +15017,13 @@
     </row>
     <row r="107">
       <c r="A107" s="10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D107" s="10" t="s">
         <v>358</v>
@@ -15079,13 +15067,13 @@
     </row>
     <row r="108">
       <c r="A108" s="10" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D108" s="10" t="s">
         <v>34</v>
@@ -15129,13 +15117,13 @@
     </row>
     <row r="109">
       <c r="A109" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>455</v>
+      </c>
+      <c r="C109" s="10" t="s">
         <v>456</v>
-      </c>
-      <c r="B109" s="16" t="s">
-        <v>457</v>
-      </c>
-      <c r="C109" s="10" t="s">
-        <v>458</v>
       </c>
       <c r="D109" s="10" t="s">
         <v>178</v>
@@ -15179,13 +15167,13 @@
     </row>
     <row r="110">
       <c r="A110" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D110" s="10" t="s">
         <v>294</v>
@@ -15229,13 +15217,13 @@
     </row>
     <row r="111">
       <c r="A111" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="C111" s="10" t="s">
         <v>461</v>
-      </c>
-      <c r="B111" s="16" t="s">
-        <v>462</v>
-      </c>
-      <c r="C111" s="10" t="s">
-        <v>463</v>
       </c>
       <c r="D111" s="10" t="s">
         <v>148</v>
@@ -15279,13 +15267,13 @@
     </row>
     <row r="112">
       <c r="A112" s="10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D112" s="10" t="s">
         <v>159</v>
@@ -15307,7 +15295,7 @@
         <v>44671.0</v>
       </c>
       <c r="M112" s="10" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="N112" s="10" t="s">
         <v>47</v>
@@ -15331,16 +15319,16 @@
     </row>
     <row r="113">
       <c r="A113" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="C113" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="B113" s="16" t="s">
+      <c r="D113" s="10" t="s">
         <v>468</v>
-      </c>
-      <c r="C113" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="D113" s="10" t="s">
-        <v>470</v>
       </c>
       <c r="E113" s="10" t="s">
         <v>19</v>
@@ -15381,13 +15369,13 @@
     </row>
     <row r="114">
       <c r="A114" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D114" s="10" t="s">
         <v>297</v>
@@ -15431,13 +15419,13 @@
     </row>
     <row r="115">
       <c r="A115" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="B115" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="C115" s="10" t="s">
         <v>473</v>
-      </c>
-      <c r="B115" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="C115" s="10" t="s">
-        <v>475</v>
       </c>
       <c r="D115" s="10" t="s">
         <v>145</v>
@@ -15447,7 +15435,7 @@
       </c>
       <c r="F115" s="12"/>
       <c r="G115" s="12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H115" s="12"/>
       <c r="I115" s="12"/>
@@ -15483,13 +15471,13 @@
     </row>
     <row r="116">
       <c r="A116" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>476</v>
+      </c>
+      <c r="C116" s="10" t="s">
         <v>477</v>
-      </c>
-      <c r="B116" s="16" t="s">
-        <v>478</v>
-      </c>
-      <c r="C116" s="10" t="s">
-        <v>479</v>
       </c>
       <c r="D116" s="10" t="s">
         <v>219</v>
@@ -15533,13 +15521,13 @@
     </row>
     <row r="117">
       <c r="A117" s="10" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D117" s="10" t="s">
         <v>213</v>
@@ -15549,7 +15537,7 @@
       </c>
       <c r="F117" s="12"/>
       <c r="G117" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
@@ -15585,13 +15573,13 @@
     </row>
     <row r="118">
       <c r="A118" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="C118" s="10" t="s">
         <v>483</v>
-      </c>
-      <c r="B118" s="16" t="s">
-        <v>484</v>
-      </c>
-      <c r="C118" s="10" t="s">
-        <v>485</v>
       </c>
       <c r="D118" s="10" t="s">
         <v>178</v>
@@ -15635,13 +15623,13 @@
     </row>
     <row r="119">
       <c r="A119" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="C119" s="10" t="s">
         <v>486</v>
-      </c>
-      <c r="B119" s="16" t="s">
-        <v>487</v>
-      </c>
-      <c r="C119" s="10" t="s">
-        <v>488</v>
       </c>
       <c r="D119" s="10" t="s">
         <v>201</v>
@@ -15685,13 +15673,13 @@
     </row>
     <row r="120">
       <c r="A120" s="10" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D120" s="10" t="s">
         <v>300</v>
@@ -15735,16 +15723,16 @@
     </row>
     <row r="121">
       <c r="A121" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="C121" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="D121" s="10" t="s">
         <v>492</v>
-      </c>
-      <c r="C121" s="10" t="s">
-        <v>493</v>
-      </c>
-      <c r="D121" s="10" t="s">
-        <v>494</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>19</v>
@@ -15785,16 +15773,16 @@
     </row>
     <row r="122">
       <c r="A122" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="C122" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="B122" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="C122" s="10" t="s">
-        <v>497</v>
-      </c>
       <c r="D122" s="10" t="s">
-        <v>498</v>
+        <v>397</v>
       </c>
       <c r="E122" s="10" t="s">
         <v>19</v>
@@ -15835,16 +15823,16 @@
     </row>
     <row r="123">
       <c r="A123" s="10" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D123" s="10" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E123" s="10" t="s">
         <v>19</v>
@@ -15885,13 +15873,13 @@
     </row>
     <row r="124">
       <c r="A124" s="10" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D124" s="10" t="s">
         <v>159</v>
@@ -15931,23 +15919,23 @@
     </row>
     <row r="125">
       <c r="A125" s="10" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D125" s="10" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F125" s="12"/>
       <c r="G125" s="12" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="H125" s="12"/>
       <c r="I125" s="12"/>
@@ -15983,13 +15971,13 @@
     </row>
     <row r="126">
       <c r="A126" s="10" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C126" s="32" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D126" s="10" t="s">
         <v>300</v>
@@ -16033,13 +16021,13 @@
     </row>
     <row r="127">
       <c r="A127" s="10" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D127" s="10" t="s">
         <v>358</v>
@@ -16083,13 +16071,13 @@
     </row>
     <row r="128">
       <c r="A128" s="10" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D128" s="10" t="s">
         <v>378</v>
@@ -16133,13 +16121,13 @@
     </row>
     <row r="129">
       <c r="A129" s="10" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C129" s="32" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D129" s="10" t="s">
         <v>300</v>
@@ -16183,16 +16171,16 @@
     </row>
     <row r="130">
       <c r="A130" s="10" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C130" s="10" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D130" s="10" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E130" s="10" t="s">
         <v>19</v>
@@ -16231,16 +16219,16 @@
     </row>
     <row r="131">
       <c r="A131" s="10" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C131" s="10" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D131" s="10" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E131" s="10" t="s">
         <v>19</v>
@@ -16281,13 +16269,13 @@
     </row>
     <row r="132">
       <c r="A132" s="39" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C132" s="39" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D132" s="36" t="s">
         <v>121</v>
@@ -16300,7 +16288,7 @@
       <c r="H132" s="34"/>
       <c r="I132" s="34"/>
       <c r="J132" s="17" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="K132" s="35">
         <v>44139.0</v>
@@ -16331,16 +16319,16 @@
     </row>
     <row r="133">
       <c r="A133" s="39" t="s">
+        <v>523</v>
+      </c>
+      <c r="B133" s="40" t="s">
+        <v>524</v>
+      </c>
+      <c r="C133" s="36" t="s">
+        <v>525</v>
+      </c>
+      <c r="D133" s="36" t="s">
         <v>526</v>
-      </c>
-      <c r="B133" s="40" t="s">
-        <v>527</v>
-      </c>
-      <c r="C133" s="36" t="s">
-        <v>528</v>
-      </c>
-      <c r="D133" s="36" t="s">
-        <v>529</v>
       </c>
       <c r="E133" s="10" t="s">
         <v>19</v>
@@ -16350,7 +16338,7 @@
       <c r="H133" s="34"/>
       <c r="I133" s="34"/>
       <c r="J133" s="17" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="K133" s="35">
         <v>44139.0</v>
@@ -16381,16 +16369,16 @@
     </row>
     <row r="134">
       <c r="A134" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="B134" s="40" t="s">
+        <v>529</v>
+      </c>
+      <c r="C134" s="39" t="s">
+        <v>530</v>
+      </c>
+      <c r="D134" s="36" t="s">
         <v>531</v>
-      </c>
-      <c r="B134" s="40" t="s">
-        <v>532</v>
-      </c>
-      <c r="C134" s="39" t="s">
-        <v>533</v>
-      </c>
-      <c r="D134" s="36" t="s">
-        <v>534</v>
       </c>
       <c r="E134" s="10" t="s">
         <v>19</v>
@@ -16400,7 +16388,7 @@
       <c r="H134" s="34"/>
       <c r="I134" s="34"/>
       <c r="J134" s="17" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="K134" s="35">
         <v>44139.0</v>
@@ -16431,16 +16419,16 @@
     </row>
     <row r="135">
       <c r="A135" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="C135" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="D135" s="10" t="s">
         <v>536</v>
-      </c>
-      <c r="B135" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="C135" s="10" t="s">
-        <v>538</v>
-      </c>
-      <c r="D135" s="10" t="s">
-        <v>539</v>
       </c>
       <c r="E135" s="10" t="s">
         <v>19</v>
@@ -16479,13 +16467,13 @@
     </row>
     <row r="136">
       <c r="A136" s="10" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C136" s="10" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D136" s="10" t="s">
         <v>159</v>
@@ -16527,13 +16515,13 @@
     </row>
     <row r="137">
       <c r="A137" s="10" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D137" s="10" t="s">
         <v>145</v>
@@ -16577,13 +16565,13 @@
     </row>
     <row r="138">
       <c r="A138" s="10" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="D138" s="10" t="s">
         <v>198</v>
@@ -16627,16 +16615,16 @@
     </row>
     <row r="139">
       <c r="A139" s="10" t="s">
+        <v>545</v>
+      </c>
+      <c r="B139" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="D139" s="10" t="s">
         <v>548</v>
-      </c>
-      <c r="B139" s="16" t="s">
-        <v>549</v>
-      </c>
-      <c r="C139" s="10" t="s">
-        <v>550</v>
-      </c>
-      <c r="D139" s="10" t="s">
-        <v>551</v>
       </c>
       <c r="E139" s="10" t="s">
         <v>19</v>
@@ -16677,13 +16665,13 @@
     </row>
     <row r="140">
       <c r="A140" s="10" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D140" s="10" t="s">
         <v>319</v>
@@ -16727,13 +16715,13 @@
     </row>
     <row r="141">
       <c r="A141" s="10" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D141" s="10" t="s">
         <v>159</v>
@@ -16743,7 +16731,7 @@
       </c>
       <c r="F141" s="12"/>
       <c r="G141" s="12" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="H141" s="12"/>
       <c r="I141" s="12"/>
@@ -16779,16 +16767,16 @@
     </row>
     <row r="142">
       <c r="A142" s="10" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C142" s="10" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D142" s="10" t="s">
-        <v>498</v>
+        <v>397</v>
       </c>
       <c r="E142" s="10" t="s">
         <v>19</v>
@@ -16829,16 +16817,16 @@
     </row>
     <row r="143">
       <c r="A143" s="10" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D143" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E143" s="10" t="s">
         <v>19</v>
@@ -16879,16 +16867,16 @@
     </row>
     <row r="144">
       <c r="A144" s="10" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B144" s="16" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E144" s="10" t="s">
         <v>19</v>
@@ -16929,13 +16917,13 @@
     </row>
     <row r="145">
       <c r="A145" s="10" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B145" s="16" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D145" s="10" t="s">
         <v>127</v>
@@ -16979,16 +16967,16 @@
     </row>
     <row r="146">
       <c r="A146" s="10" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B146" s="16" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C146" s="10" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D146" s="10" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E146" s="10" t="s">
         <v>19</v>
@@ -17029,23 +17017,23 @@
     </row>
     <row r="147">
       <c r="A147" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="B147" s="16" t="s">
+        <v>570</v>
+      </c>
+      <c r="C147" s="10" t="s">
+        <v>571</v>
+      </c>
+      <c r="D147" s="10" t="s">
         <v>572</v>
-      </c>
-      <c r="B147" s="16" t="s">
-        <v>573</v>
-      </c>
-      <c r="C147" s="10" t="s">
-        <v>574</v>
-      </c>
-      <c r="D147" s="10" t="s">
-        <v>575</v>
       </c>
       <c r="E147" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F147" s="12"/>
       <c r="G147" s="12" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="H147" s="12"/>
       <c r="I147" s="12"/>
@@ -17081,16 +17069,16 @@
     </row>
     <row r="148">
       <c r="A148" s="10" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E148" s="10" t="s">
         <v>19</v>
@@ -17111,7 +17099,7 @@
         <v>30</v>
       </c>
       <c r="O148" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P148" s="12"/>
       <c r="Q148" s="12"/>
@@ -17129,13 +17117,13 @@
     </row>
     <row r="149">
       <c r="A149" s="10" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B149" s="16" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D149" s="10" t="s">
         <v>148</v>
@@ -17145,7 +17133,7 @@
       </c>
       <c r="F149" s="12"/>
       <c r="G149" s="12" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="H149" s="12"/>
       <c r="I149" s="12"/>
@@ -17181,13 +17169,13 @@
     </row>
     <row r="150">
       <c r="A150" s="10" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B150" s="16" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D150" s="10" t="s">
         <v>174</v>
@@ -17231,13 +17219,13 @@
     </row>
     <row r="151">
       <c r="A151" s="10" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B151" s="16" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D151" s="10" t="s">
         <v>358</v>
@@ -17281,13 +17269,13 @@
     </row>
     <row r="152">
       <c r="A152" s="10" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D152" s="10" t="s">
         <v>371</v>
@@ -17331,13 +17319,13 @@
     </row>
     <row r="153">
       <c r="A153" s="10" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B153" s="16" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D153" s="10" t="s">
         <v>204</v>
@@ -17381,13 +17369,13 @@
     </row>
     <row r="154">
       <c r="A154" s="10" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C154" s="10" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D154" s="10" t="s">
         <v>294</v>
@@ -17431,13 +17419,13 @@
     </row>
     <row r="155">
       <c r="A155" s="10" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B155" s="16" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D155" s="10" t="s">
         <v>294</v>
@@ -17481,13 +17469,13 @@
     </row>
     <row r="156">
       <c r="A156" s="10" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B156" s="16" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D156" s="10" t="s">
         <v>294</v>
@@ -17531,13 +17519,13 @@
     </row>
     <row r="157">
       <c r="A157" s="10" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B157" s="11" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D157" s="10" t="s">
         <v>34</v>
@@ -17579,16 +17567,16 @@
     </row>
     <row r="158">
       <c r="A158" s="10" t="s">
+        <v>600</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>601</v>
+      </c>
+      <c r="C158" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="D158" s="10" t="s">
         <v>603</v>
-      </c>
-      <c r="B158" s="11" t="s">
-        <v>604</v>
-      </c>
-      <c r="C158" s="10" t="s">
-        <v>605</v>
-      </c>
-      <c r="D158" s="10" t="s">
-        <v>606</v>
       </c>
       <c r="E158" s="10" t="s">
         <v>19</v>
@@ -17621,16 +17609,16 @@
     </row>
     <row r="159">
       <c r="A159" s="10" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B159" s="11" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D159" s="10" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E159" s="10" t="s">
         <v>19</v>
@@ -17663,13 +17651,13 @@
     </row>
     <row r="160">
       <c r="A160" s="10" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B160" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C160" s="10" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D160" s="10" t="s">
         <v>204</v>
@@ -17713,16 +17701,16 @@
     </row>
     <row r="161">
       <c r="A161" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="B161" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="C161" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="D161" s="10" t="s">
         <v>613</v>
-      </c>
-      <c r="B161" s="11" t="s">
-        <v>614</v>
-      </c>
-      <c r="C161" s="10" t="s">
-        <v>615</v>
-      </c>
-      <c r="D161" s="10" t="s">
-        <v>616</v>
       </c>
       <c r="E161" s="10" t="s">
         <v>19</v>
@@ -17761,13 +17749,13 @@
     </row>
     <row r="162">
       <c r="A162" s="10" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B162" s="16" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D162" s="10" t="s">
         <v>219</v>
@@ -17777,7 +17765,7 @@
       </c>
       <c r="F162" s="10"/>
       <c r="G162" s="10" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="H162" s="12"/>
       <c r="I162" s="12"/>
@@ -17813,13 +17801,13 @@
     </row>
     <row r="163">
       <c r="A163" s="10" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="B163" s="16" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D163" s="10" t="s">
         <v>219</v>
@@ -17863,13 +17851,13 @@
     </row>
     <row r="164">
       <c r="A164" s="10" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B164" s="16" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D164" s="10" t="s">
         <v>339</v>
@@ -17913,13 +17901,13 @@
     </row>
     <row r="165">
       <c r="A165" s="10" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B165" s="16" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D165" s="10" t="s">
         <v>294</v>
@@ -17963,13 +17951,13 @@
     </row>
     <row r="166">
       <c r="A166" s="10" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="B166" s="16" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C166" s="10" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D166" s="10" t="s">
         <v>355</v>
@@ -18013,13 +18001,13 @@
     </row>
     <row r="167">
       <c r="A167" s="10" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B167" s="11" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D167" s="10" t="s">
         <v>145</v>
@@ -18061,16 +18049,16 @@
     </row>
     <row r="168">
       <c r="A168" s="10" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B168" s="16" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D168" s="10" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E168" s="10" t="s">
         <v>19</v>
@@ -18111,16 +18099,16 @@
     </row>
     <row r="169">
       <c r="A169" s="10" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="B169" s="16" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D169" s="10" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E169" s="10" t="s">
         <v>19</v>
@@ -18161,13 +18149,13 @@
     </row>
     <row r="170">
       <c r="A170" s="10" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B170" s="16" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D170" s="10" t="s">
         <v>345</v>
@@ -18211,13 +18199,13 @@
     </row>
     <row r="171">
       <c r="A171" s="10" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B171" s="16" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D171" s="10" t="s">
         <v>170</v>
@@ -18261,13 +18249,13 @@
     </row>
     <row r="172">
       <c r="A172" s="10" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B172" s="16" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C172" s="10" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D172" s="10" t="s">
         <v>294</v>
@@ -18311,13 +18299,13 @@
     </row>
     <row r="173">
       <c r="A173" s="10" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B173" s="16" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D173" s="10" t="s">
         <v>219</v>
@@ -18361,13 +18349,13 @@
     </row>
     <row r="174">
       <c r="A174" s="10" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B174" s="16" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D174" s="10" t="s">
         <v>294</v>
@@ -18411,16 +18399,16 @@
     </row>
     <row r="175">
       <c r="A175" s="10" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B175" s="16" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E175" s="10" t="s">
         <v>19</v>
@@ -18461,13 +18449,13 @@
     </row>
     <row r="176">
       <c r="A176" s="10" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C176" s="10" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="D176" s="10" t="s">
         <v>145</v>
@@ -18480,7 +18468,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="12"/>
       <c r="J176" s="19" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="K176" s="13">
         <v>43795.0</v>
@@ -18490,10 +18478,10 @@
         <v>21</v>
       </c>
       <c r="N176" s="10" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="O176" s="14" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="P176" s="12"/>
       <c r="Q176" s="12"/>
@@ -18511,16 +18499,16 @@
     </row>
     <row r="177">
       <c r="A177" s="10" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B177" s="16" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E177" s="10" t="s">
         <v>19</v>
@@ -18561,13 +18549,13 @@
     </row>
     <row r="178">
       <c r="A178" s="10" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B178" s="16" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C178" s="10" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D178" s="10" t="s">
         <v>371</v>
@@ -18611,13 +18599,13 @@
     </row>
     <row r="179">
       <c r="A179" s="10" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="B179" s="16" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D179" s="10" t="s">
         <v>371</v>
@@ -18661,13 +18649,13 @@
     </row>
     <row r="180">
       <c r="A180" s="10" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="B180" s="16" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C180" s="32" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D180" s="10" t="s">
         <v>300</v>
@@ -18711,13 +18699,13 @@
     </row>
     <row r="181">
       <c r="A181" s="10" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B181" s="16" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="D181" s="10" t="s">
         <v>127</v>
@@ -18761,13 +18749,13 @@
     </row>
     <row r="182">
       <c r="A182" s="10" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B182" s="16" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D182" s="10" t="s">
         <v>34</v>
@@ -18811,13 +18799,13 @@
     </row>
     <row r="183">
       <c r="A183" s="10" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="B183" s="16" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C183" s="32" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D183" s="10" t="s">
         <v>330</v>
@@ -18827,7 +18815,7 @@
       </c>
       <c r="F183" s="12"/>
       <c r="G183" s="12" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="H183" s="12"/>
       <c r="I183" s="12"/>
@@ -18863,13 +18851,13 @@
     </row>
     <row r="184">
       <c r="A184" s="10" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D184" s="10" t="s">
         <v>330</v>
@@ -18911,13 +18899,13 @@
     </row>
     <row r="185">
       <c r="A185" s="10" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B185" s="16" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="D185" s="10" t="s">
         <v>204</v>
@@ -18961,13 +18949,13 @@
     </row>
     <row r="186">
       <c r="A186" s="10" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="B186" s="16" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D186" s="10" t="s">
         <v>201</v>
@@ -19011,13 +18999,13 @@
     </row>
     <row r="187">
       <c r="A187" s="10" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="B187" s="16" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C187" s="10" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D187" s="10" t="s">
         <v>127</v>
@@ -19061,13 +19049,13 @@
     </row>
     <row r="188">
       <c r="A188" s="10" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B188" s="16" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D188" s="10" t="s">
         <v>219</v>
@@ -19111,13 +19099,13 @@
     </row>
     <row r="189">
       <c r="A189" s="10" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="B189" s="16" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D189" s="10" t="s">
         <v>319</v>
@@ -19161,16 +19149,16 @@
     </row>
     <row r="190">
       <c r="A190" s="32" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="B190" s="44" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="E190" s="10" t="s">
         <v>19</v>
@@ -19211,13 +19199,13 @@
     </row>
     <row r="191">
       <c r="A191" s="10" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="B191" s="16" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="D191" s="10" t="s">
         <v>34</v>
@@ -19261,16 +19249,16 @@
     </row>
     <row r="192">
       <c r="A192" s="10" t="s">
+        <v>693</v>
+      </c>
+      <c r="B192" s="11" t="s">
+        <v>694</v>
+      </c>
+      <c r="C192" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="D192" s="10" t="s">
         <v>696</v>
-      </c>
-      <c r="B192" s="11" t="s">
-        <v>697</v>
-      </c>
-      <c r="C192" s="10" t="s">
-        <v>698</v>
-      </c>
-      <c r="D192" s="10" t="s">
-        <v>699</v>
       </c>
       <c r="E192" s="10" t="s">
         <v>19</v>
@@ -19291,7 +19279,7 @@
         <v>30</v>
       </c>
       <c r="O192" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P192" s="12"/>
       <c r="Q192" s="12"/>
@@ -19309,13 +19297,13 @@
     </row>
     <row r="193">
       <c r="A193" s="10" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="B193" s="28" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D193" s="10" t="s">
         <v>219</v>
@@ -19359,13 +19347,13 @@
     </row>
     <row r="194">
       <c r="A194" s="10" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="B194" s="16" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D194" s="10" t="s">
         <v>378</v>
@@ -19409,13 +19397,13 @@
     </row>
     <row r="195">
       <c r="A195" s="10" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="B195" s="11" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="C195" s="10" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="D195" s="10" t="s">
         <v>170</v>
@@ -19457,16 +19445,16 @@
     </row>
     <row r="196">
       <c r="A196" s="10" t="s">
+        <v>704</v>
+      </c>
+      <c r="B196" s="11" t="s">
+        <v>705</v>
+      </c>
+      <c r="C196" s="10" t="s">
+        <v>706</v>
+      </c>
+      <c r="D196" s="10" t="s">
         <v>707</v>
-      </c>
-      <c r="B196" s="11" t="s">
-        <v>708</v>
-      </c>
-      <c r="C196" s="10" t="s">
-        <v>709</v>
-      </c>
-      <c r="D196" s="10" t="s">
-        <v>710</v>
       </c>
       <c r="E196" s="10" t="s">
         <v>19</v>
@@ -19476,7 +19464,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="12"/>
       <c r="J196" s="19" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="K196" s="13">
         <v>43795.0</v>
@@ -19486,10 +19474,10 @@
         <v>21</v>
       </c>
       <c r="N196" s="10" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="O196" s="14" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="P196" s="12"/>
       <c r="Q196" s="12"/>
@@ -19507,23 +19495,23 @@
     </row>
     <row r="197">
       <c r="A197" s="10" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="B197" s="16" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="C197" s="10" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="D197" s="10" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E197" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F197" s="10"/>
       <c r="G197" s="10" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="H197" s="12"/>
       <c r="I197" s="12"/>
@@ -19559,13 +19547,13 @@
     </row>
     <row r="198">
       <c r="A198" s="10" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B198" s="25" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="C198" s="45" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="D198" s="25" t="s">
         <v>213</v>
@@ -19607,16 +19595,16 @@
     </row>
     <row r="199">
       <c r="A199" s="10" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B199" s="16" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E199" s="10" t="s">
         <v>19</v>
@@ -19657,16 +19645,16 @@
     </row>
     <row r="200">
       <c r="A200" s="10" t="s">
+        <v>717</v>
+      </c>
+      <c r="B200" s="11" t="s">
+        <v>718</v>
+      </c>
+      <c r="C200" s="10" t="s">
+        <v>719</v>
+      </c>
+      <c r="D200" s="10" t="s">
         <v>720</v>
-      </c>
-      <c r="B200" s="11" t="s">
-        <v>721</v>
-      </c>
-      <c r="C200" s="10" t="s">
-        <v>722</v>
-      </c>
-      <c r="D200" s="10" t="s">
-        <v>723</v>
       </c>
       <c r="E200" s="10" t="s">
         <v>19</v>
@@ -19705,16 +19693,16 @@
     </row>
     <row r="201">
       <c r="A201" s="10" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B201" s="11" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C201" s="10" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="D201" s="10" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="E201" s="10" t="s">
         <v>19</v>
@@ -19753,13 +19741,13 @@
     </row>
     <row r="202">
       <c r="A202" s="10" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B202" s="11" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="C202" s="10" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="D202" s="10" t="s">
         <v>159</v>
@@ -19801,16 +19789,16 @@
     </row>
     <row r="203">
       <c r="A203" s="10" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B203" s="11" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="C203" s="10" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="D203" s="10" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="E203" s="10" t="s">
         <v>19</v>
@@ -19849,16 +19837,16 @@
     </row>
     <row r="204">
       <c r="A204" s="10" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="B204" s="11" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="C204" s="10" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="E204" s="10" t="s">
         <v>19</v>
@@ -19897,13 +19885,13 @@
     </row>
     <row r="205">
       <c r="A205" s="10" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="B205" s="16" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="C205" s="32" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="D205" s="10" t="s">
         <v>330</v>
@@ -19947,13 +19935,13 @@
     </row>
     <row r="206">
       <c r="A206" s="10" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B206" s="16" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C206" s="10" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D206" s="10" t="s">
         <v>330</v>
@@ -19997,13 +19985,13 @@
     </row>
     <row r="207">
       <c r="A207" s="10" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B207" s="16" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C207" s="10" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="D207" s="10" t="s">
         <v>127</v>
@@ -20047,13 +20035,13 @@
     </row>
     <row r="208">
       <c r="A208" s="10" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="B208" s="11" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="C208" s="10" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="D208" s="10" t="s">
         <v>294</v>
@@ -20095,13 +20083,13 @@
     </row>
     <row r="209">
       <c r="A209" s="10" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B209" s="16" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C209" s="10" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D209" s="10" t="s">
         <v>294</v>
@@ -20148,7 +20136,7 @@
     </row>
     <row r="211">
       <c r="A211" s="10" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B211" s="45"/>
       <c r="C211" s="25"/>
@@ -20182,7 +20170,7 @@
     </row>
     <row r="212">
       <c r="A212" s="10" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B212" s="25"/>
       <c r="C212" s="47"/>
@@ -20216,7 +20204,7 @@
     </row>
     <row r="213">
       <c r="A213" s="10" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="B213" s="47"/>
       <c r="C213" s="25"/>
@@ -20250,7 +20238,7 @@
     </row>
     <row r="214">
       <c r="A214" s="10" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="B214" s="28"/>
       <c r="C214" s="12"/>
@@ -20284,7 +20272,7 @@
     </row>
     <row r="215">
       <c r="A215" s="10" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="B215" s="28"/>
       <c r="C215" s="12"/>
@@ -20321,7 +20309,7 @@
     </row>
     <row r="217">
       <c r="A217" s="10" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="B217" s="28"/>
     </row>

</xml_diff>